<commit_message>
mettre à jour BDD
</commit_message>
<xml_diff>
--- a/autre/bd/Base_de_donnees_suisse_des_valeurs_nutritives_V6.4.xlsx
+++ b/autre/bd/Base_de_donnees_suisse_des_valeurs_nutritives_V6.4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\下载\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - Efrei\Efrei\S6.5 Matercamp\Projet\Eat-well\autre\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A762AF7-AA18-42FB-8EB5-860BCCB8A005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8D0F27-9E84-4ECA-85BE-55E3330993C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5625" uniqueCount="1675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5625" uniqueCount="1678">
   <si>
     <t>ID</t>
   </si>
@@ -4241,817 +4241,830 @@
     <t>Eau minérale Vichy-Célestins</t>
   </si>
   <si>
+    <t>Eau minérale Zurzacher</t>
+  </si>
+  <si>
+    <t>Eichhof Hubertus (bière spéciale brune, 6 vol%)</t>
+  </si>
+  <si>
+    <t>Energy drink, avec édulcorants (Moyenne de produits du commerce)</t>
+  </si>
+  <si>
+    <t>Ittinger (bière spéciale ambre, 5.6 vol%)</t>
+  </si>
+  <si>
+    <t>Malibu Coconut (21 vol%)</t>
+  </si>
+  <si>
+    <t>Pastis 51 de Marseille (45 vol%)</t>
+  </si>
+  <si>
+    <t>Sauce Worcester (Moyenne de produits du commerce)</t>
+  </si>
+  <si>
+    <t>Sucre vanillé (Moyenne de produits du commerce)</t>
+  </si>
+  <si>
+    <t>1662;1682</t>
+  </si>
+  <si>
+    <t>Suze (20 vol%)</t>
+  </si>
+  <si>
+    <t>Yogourt, à la grecque, avec crème, nature (Moyenne de produits du commerce)</t>
+  </si>
+  <si>
+    <t>Aargauer Zentralmolkerei AG, Suhr, Schweiz</t>
+  </si>
+  <si>
+    <t>Agroscope Liebefeld-Posieux, Liebefeld, Schweiz</t>
+  </si>
+  <si>
+    <t>Banca dati di composizione degli alimenti per studi epidemiologici in Italia</t>
+  </si>
+  <si>
+    <t>Bischofszell Nahrungsmittel AG, Bischofszell, Schweiz</t>
+  </si>
+  <si>
+    <t>Bundeslebensmittelschlüssel, BLS II.3.1, Karlsruhe, Deutschland</t>
+  </si>
+  <si>
+    <t>Bundeslebensmittelschlüssel, Karlsruhe, Deutschland</t>
+  </si>
+  <si>
+    <t>Canadian Nutrient File, version 2005. http://webprod.hc-sc.gc.ca/cnf-fce/start-debuter.do?lang=eng</t>
+  </si>
+  <si>
+    <t>Coop Schweiz, Zentrallabor, Pratteln, Schweiz</t>
+  </si>
+  <si>
+    <t>Danish food composition table</t>
+  </si>
+  <si>
+    <t>Emmi Schweiz AG, Emmen, Schweiz</t>
+  </si>
+  <si>
+    <t>Feldschlösschen Getränke AG, Rheinfelden, Schweiz</t>
+  </si>
+  <si>
+    <t>Haco AG, Gümlingen, Schweiz</t>
+  </si>
+  <si>
+    <t>Institut für Lebensmittel- und Ernährungswissenschaften, ETH Zürich, Schweiz 1</t>
+  </si>
+  <si>
+    <t>Institut für Lebensmittel- und Ernährungswissenschaften, ETH Zürich, Schweiz 2</t>
+  </si>
+  <si>
+    <t>Institut für Nutztierwissenschaften, ETH Zürich, Schweiz</t>
+  </si>
+  <si>
+    <t>Institute of Nutrition, Nakorn Pathom, Thailand</t>
+  </si>
+  <si>
+    <t>Kantonales Labor Zürich, Schweiz</t>
+  </si>
+  <si>
+    <t>Midor AG, Meilen, Schweiz</t>
+  </si>
+  <si>
+    <t>Mifa AG, Frenkendorf, Schweiz</t>
+  </si>
+  <si>
+    <t>Møller et al. Danish Food Composition Databank, revision 6.0. Food Informatics, Department of Nutrition, Danish Institute for Food and Veterinary Research. June 2005. www.foodcomp.dk/</t>
+  </si>
+  <si>
+    <t>Nährwerttabellen für Milch und Milchprodukte, Renner &amp; Renz-Schauen, Giessen, Deutschland</t>
+  </si>
+  <si>
+    <t>Nährwerttabellen, Souci Fachmann Kraut, Garching, Deutschland</t>
+  </si>
+  <si>
+    <t>Nestlé Suisse SA, Hirzel, Schweiz</t>
+  </si>
+  <si>
+    <t>Nestlé Suisse SA, Vevey, Schweiz</t>
+  </si>
+  <si>
+    <t>Nutrilait SA, Plan les Ouates, Schweiz</t>
+  </si>
+  <si>
+    <t>Répértoire général des aliments, Paris, Frankreich</t>
+  </si>
+  <si>
+    <t>Rivella AG, Rothrist, Schweiz</t>
+  </si>
+  <si>
+    <t>Schokoladefabriken Lindt &amp; Sprüngli AG, Produktinformationen Schokolade, Kilchberg, Schweiz, 2008.</t>
+  </si>
+  <si>
+    <t>Schweizerisches Vitamininstitut, Basel, Schweiz</t>
+  </si>
+  <si>
+    <t>Swiss Mill, Zürich, Schweiz</t>
+  </si>
+  <si>
+    <t>Swiss Quality Testing Services SQTS, Dietikon, Schweiz</t>
+  </si>
+  <si>
+    <t>SwissFIR, DAGRL, ETH Zürich, Schweiz</t>
+  </si>
+  <si>
+    <t>The composition of foods, McCance &amp; Widdowson</t>
+  </si>
+  <si>
+    <t>UFAG Laboratorien AG, Sursee, Schweiz</t>
+  </si>
+  <si>
+    <t>USDA National Nutrient Database for Standard Reference, Release 16, Beltsville, USA</t>
+  </si>
+  <si>
+    <t>USDA National Nutrient Database for Standard Reference, Release 19, Beltsville, USA. www.nal.usda.gov/fnic/foodcomp/search/</t>
+  </si>
+  <si>
+    <t>AFSSA/CIQUAL French food composition table version 2008. www.afssa.fr/TableCIQUAL/</t>
+  </si>
+  <si>
+    <t>Banca Dati di Composizione degli Alimenti INRAN, 2007. www.inran.it/646/tabelle_di_composizione_degli_alimenti.html</t>
+  </si>
+  <si>
+    <t>Barros et al. Chemical Composition and Biological Properties of Portuguese Wild Mushrooms: A Comprehensive Study. J. Agric. Food Chem. 56(10):3856-3862, 2008.</t>
+  </si>
+  <si>
+    <t>Borges et al. Nutritional quality of chestnut  (Castanea sativa Mill.) cultivars from Portugal. Food Chemistry 106:976-984, 2008.</t>
+  </si>
+  <si>
+    <t>Bureau et al. HPLC Determination of Carotenoids in Fruits and Vegetables in the United States. Journal of Food Science 51: 128-130, 1986.</t>
+  </si>
+  <si>
+    <t>Cabrera et al. Mineral content in legumes and nuts: contribution to the Spanish dietary intake. The science of the Total Enviroment 308:1-14, 2003.</t>
+  </si>
+  <si>
+    <t>Cardozo, Li. Total Dietary Fiber Content of Selected Nuts by Two Enzymatic-Gravimetric Methods. Journal of Food Composition and Analysis 7: 37-43, 1994.</t>
+  </si>
+  <si>
+    <t>De Oliveira, Rodriguez-Amaya. Processed and prepared corn products as sources of lutein and zeaxanthin: compositional variation in the food chain. J.Food Sci. 72(1):S79-S85, 2007.</t>
+  </si>
+  <si>
+    <t>Dias et al. Carotenoids in traditional Portuguese fruits and vegetables. Food Chemistry 113:808-815, 2009.</t>
+  </si>
+  <si>
+    <t>EL-Qudah. Identification and Quantification of Major Carotenoids in Some Vegetables. American Journal of Applied Sciences 6:492-497, 2009.</t>
+  </si>
+  <si>
+    <t>Food Composition Database for Epidemiological Studies in Italy by Gnagnarella P, Salvini S, Parpinel M. Version 1.2008, www.ieo.it/bda</t>
+  </si>
+  <si>
+    <t>Gambelli et al. Constituents of nutritional relevance in fermented milk products in Italy. Food Chemistry 66, 353-359, 1999.</t>
+  </si>
+  <si>
+    <t>Garcia-Linares et al. Microbiological and nutritional quality of sous vide or traditionally processed fish: Influence of fat content. J.Food Qual. 27(5):371-387, 2004.</t>
+  </si>
+  <si>
+    <t>Granado et al. Carotenoid composition in raw and cooked Spanish vegetables. Journal of Agriculture and Food Chemistry 40:2135-2140, 1992.</t>
+  </si>
+  <si>
+    <t>Haldimann et al. Iodine content of food groups. Journal of Food Composition and Analysis 18:461-471, 2005.</t>
+  </si>
+  <si>
+    <t>Hart et al. Development and evaluation of an HPLC method for the analysis of carotenoids in foods, measurement of carotenoid content of vegetables and fruits consumed in UK. Food Chemistry 54:101-111, 1995.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heinonen et al. Carotenoids in Finnish foods: vegetables, fruits, and berries. Journal of Food Composition and Analysis 37:655-659, 1989. </t>
+  </si>
+  <si>
+    <t>Heinonen et al. Carotenoids and retinoids in Finnish foods: cereal and bakery products. Cereal Chem. 66(4):270-273, 1989.</t>
+  </si>
+  <si>
+    <t>Heinonen et al. Carotenoids and retinoids in Finnish foods: dietary fats. J.Food Compos.Anal. 1(4):334-340, 1988.</t>
+  </si>
+  <si>
+    <t>Högberg et al. Muscle lipids, vitamins E and A, and lipid oxidation as affected by diet and RN genotype in female and castrated male Hampshire crossbreed pigs. Meat Science 60 (4):411-420, 2002.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holden et al. Carotenoid Content of U.S. Foods: An Update of the Database. Journal of Food Composition and Analysis 12:169-199, 1999. </t>
+  </si>
+  <si>
+    <t>Hoppner et al. Total Folate, Pantothenic Acid and Biotin Content of Yogurt Products, Can. Inst. Sci. Technol. J. , 23: 223-225, 1990</t>
+  </si>
+  <si>
+    <t>Hulshof et al. Variation in retinol and carotenoid content of milk and milk products in The Netherlands. Journal of Food Composition and Analysis 19:67-75, 2006.</t>
+  </si>
+  <si>
+    <t>Kandlakunta et al. Carotene content of some common (cereals, pulses, vegetables, spices and condiments) and unconventional sources of plant origin. Food Chem. 106(1):85-89, 2008.</t>
+  </si>
+  <si>
+    <t>Kessler, Morel. Vitamin A Konzentration in Kalbslebern: Eine Praxiserhebung. Agrarforschung 5 (5):225-227, 1998.</t>
+  </si>
+  <si>
+    <t>Köksal et al. Nutrient composition of hazelnut (Corylus avellana L.) varieties cultivated in Turkey. Food Chemistry 99:509-515, 2006.</t>
+  </si>
+  <si>
+    <t>Kornsteiner et al. Tocopherols and total phenolics in 10 different nut types. Food Chemistry 98:381-387, 2006.</t>
+  </si>
+  <si>
+    <t>Kumar, Aalbersberg. Nutrient retention in foods after earth-oven cooking compared to other forms of domestic cooking. 2. Vitamins. Journal of Food Composition and Analysis 19:311-320, 2006.</t>
+  </si>
+  <si>
+    <t>Kurz et al. HPLC-DAD-MS characterisation of carotenoids from apricots and pumpkins for the evaluation of fruit product authenticity. Food Chemistry 110:522-530, 2008.</t>
+  </si>
+  <si>
+    <t>Leonhardt et al. Vitamin E content of different animal products: Influence of animal nutrition. Zeitschrift für Ernährungswissenschaft 36:23-27, 1997.</t>
+  </si>
+  <si>
+    <t>Leonhardt, Wenk. Animal species and muscle related differences in thiamine and riboflavin contents of Swiss meat. Food Chemistry 59:449-452, 1997.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leth et al. The intake of carotenoids in Denmark. European Journal of Lipid Science Technology 128-132, 2000. </t>
+  </si>
+  <si>
+    <t>Livsmedelsdatabas - Swedish Food Composition Database, Schweden. Version: 07.10.2008</t>
+  </si>
+  <si>
+    <t>Lo Fiego et al. Effect of dietary supplementation of vitamins C and E in rabbits. Meat Science 67:319-327, 2004.</t>
+  </si>
+  <si>
+    <t>Lombardi-Boccia et al. Aspects of meat quality: trace elements and B vitamins in raw and cooked meats. Journal of Food Composition and Analysis 18:39-46, 2005.</t>
+  </si>
+  <si>
+    <t>Majchrzak et al. Vitamin A content (retinol and retinyl esters) in livers of different animals. Food Chem. 98(4):704-710, 2006.</t>
+  </si>
+  <si>
+    <t>Mangels et al. Carotenoid content of fruits and vegetables: An evaluation of analytic data. Journal American Dietetic Association 93:284-296, 1993.</t>
+  </si>
+  <si>
+    <t>Mattila et al. Contents of Cholecalciferol, Ergocalciferol, and Their 25-Hydroxylated Metabolites in Milk Products and Raw Meat and Liver As Determined by HPLC. Journal of Agriculture and Food Chemistry 43:2394-2399, 1995.</t>
+  </si>
+  <si>
+    <t>Moreiras et al. Tablas de composicion de alimentos, Piramide, 2005.</t>
+  </si>
+  <si>
+    <t>Müller et al. Determination of the carotenoid content in selected vegetabels and fruit by HPLC and photodiode array detection. Z. Lebensm. Unters. Forsch. A. 204:88-94, 1997.</t>
+  </si>
+  <si>
+    <t>Müller et al. Einfluss der Verarbeitung auf die Carotinoidgehalte von Gemüsesäften. Babynahrung und Tiefkühlprodukten, Deutsche Gesellschaft für Qualitätsforschung 155-160, 1997.</t>
+  </si>
+  <si>
+    <t>Müller. Die tägliche Aufnahme von Carotinoiden aus Gesamtnahrungsproben und die Carotinoidgehalte ausgewählter Gemüse-und Obstarten. Z. Ernährungswissenschaft 35:45-50, 1996.</t>
+  </si>
+  <si>
+    <t>Munzuroglu et al. The vitamin and selenium contents of apricot fruit of different verieties cultivated in different geographical regions. Food Chem. 83:205-212, 2003.</t>
+  </si>
+  <si>
+    <t>Murkovic et al. Development of an Austrian Carotenoid Database. Journal of Food Composition and Analysis 13:435-440, 2000.</t>
+  </si>
+  <si>
+    <t>Nährwerttabellen für Milch und Milchprodukte, Renner &amp; Renz-Schauen, Giessen, Deutschland, 1994</t>
+  </si>
+  <si>
+    <t>National Public Health Institute, Nutrition Unit. Fineli. Finnish food composition database. Release 9. Helsinki 2008. www.ktl.fi/fineli/</t>
+  </si>
+  <si>
+    <t>Niizu et al., New data on the carotenoid composition of raw salad vegetables. Journal of Food Composition and Analysis 18:739-749, 2005.</t>
+  </si>
+  <si>
+    <t>O'Neill et al. A European carotenoid database to assess carotenoid intakes and its use in five-country comparative study. British Journal of Nutrition 85:499-507, 2001.</t>
+  </si>
+  <si>
+    <t>Oliveira et al. Chemical composition, and antioxidant and antimicrobial activities of three hazelnut (Corylus avellana L.) cultivars. Food and Chemical Toxicology 46:1801-1807, 2008.</t>
+  </si>
+  <si>
+    <t>Olmedilla et al. Quantitation of provitamin-A and non-Provitamin-A carotenoids in the fruits most commonly consumed in Spain. Food and Cancer Prevention 141-145, 1993.</t>
+  </si>
+  <si>
+    <t>Orban et al. Nutritional quality and safety of whitefish (Coregonus lavaretus) from Italian lakes. J.Food Compos.Anal. 19(6-7):737-746, 2006.</t>
+  </si>
+  <si>
+    <t>Penã-Mendez et al. Characterization of various chestnut cultivars by means of chemometrics approach. Food Chemistry 107:537-544, 2008.</t>
+  </si>
+  <si>
+    <t>Plessi et al. Dietary Fiber and Some Elements in Nuts and Wheat Brans. Journal of Food Composition and Analysis 12:91-96, 1999.</t>
+  </si>
+  <si>
+    <t>Purchas et al. Concentrations of vitamin D3 and 25-hydroxyvitamin D3 in raw and cooked New Zealand beef and lamb. J.Food Compos.Anal. 20 (2):90-98, 2007.</t>
+  </si>
+  <si>
+    <t>Saxholt, Christensen, Møller, Hartkopp, Hess Ygil, Hels: Danish Food Composition Databank, revision 7. Department of Nutrition, National Food Institute, Technical University of Denmark. 2008. www.foodcomp.dk/</t>
+  </si>
+  <si>
+    <t>Schweizerische Nährwerttabelle für Fleisch und Fleischwaren. Wissenschaftliche Fassung.</t>
+  </si>
+  <si>
+    <t>Scott, Bishop. Nutrient Content of Milk and Milk Products: Vitamins of the B Complex and Vitamin C in Retail Creams, Ice Creams and Milk Shakes, J. Sci. Foood Agric., 1988</t>
+  </si>
+  <si>
+    <t>Setiawan et al. Carotenoid Content of Selected Indonesian Fruits. Journal of Food Composition and Analysis 14:169-176, 2001.</t>
+  </si>
+  <si>
+    <t>Singh et al. Antioxidant phytochemicals in cabbage (Brassica oleracea L. var. Capitata). Scientia Horticulturae 108:233-237, 2006.</t>
+  </si>
+  <si>
+    <t>Singh et al. Variability of carotenes, vitamin C, E and phenolics in Brassica vegetables. Journal of Food Composition and  Analysis 20:106-112, 2007.</t>
+  </si>
+  <si>
+    <t>Su et al. Identification and quantitation of major carotenoids in selected components of the Mediterranean diet: green leafy vegetables, figs and olive oil. European Journal of Clinical Nutrition 56:1149-1154, 2002.</t>
+  </si>
+  <si>
+    <t>SwissFIR, DAGRL, ETH Zürich, Inhaltsstoffe Wasser, berechnet aus Analysedaten der grössten Schweizer Wasserversorger, Schweiz, 2008.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Norwegian Food Safety Authority, The Norwegian Directorate of Health and the University of Oslo. The Norwegian Food Composition Table 2006. www.matportalen.no/matvaretabellen </t>
+  </si>
+  <si>
+    <t>U.S. Department of Agriculture, Agricultural Research Service. 2007. USDA National Nutrient Database for Standard Reference, Release 21. www.nal.usda.gov/fnic/foodcomp/search/</t>
+  </si>
+  <si>
+    <t>Van Heerden et al. Nutrient Content of South African Chickens. Journal of Food Composition and Analysis 15:47-64, 2002.</t>
+  </si>
+  <si>
+    <t>Van Heerden et al. The nutrient composition of South African lamb (A2 grade). Journal of Food Composition and Analysis 20:671-680, 2007.</t>
+  </si>
+  <si>
+    <t>Welna et al. Investigation of major and trace elements and their distributions between lipid and non-lipid fractions in Brazil nuts by inductively coupled plasma atomic optical spectrometry. Food Chemistry 111:1012-1015, 2008.</t>
+  </si>
+  <si>
+    <t>Williams et al. Composition of Australian red meat 2002. 3. Nutrient profile, Food Australia 59(7), 331-341, 2007.</t>
+  </si>
+  <si>
+    <t>Yano et al. Quantitation of Carotenoids in Raw and Processed Fruits in Japan. Food Sci. Technol. Res. 11:13-18, 2005.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Voll-, Halb- und Kaffeerahm, Mitt. Gebiete Lebensm. Hyg. 87:103-110, 1996.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer konsumreifer Emmentaler, Greyerzer, Sbrinz, Appenzeller und Tilsiter, Schweiz. Milchw. Forschung 17:109-118, 1988.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Joghurt, Mitt. Gebiete Lebensm. Hyg. 87:743-754, 1996.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer Milch, Mitt. Gebiete Lebensm. Hyg. 90:135-148, 1999.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer Butter, Mitt. Gebiete Lebensm. Hyg. 89:84-96, 1998.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Quark und Hüttenkäse, Mitt. Gebiete Lebensm. Hyg. 90:662-669, 1999.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung schweizerischer konsumreifer Weich- und Halbhartkäse, Mitt. Gebierte Lebensm. Hyg. 85:366-381, 1994.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Ziger, Mitt. Gebiete Lebensm. Hyg. 89:294-300, 1998.</t>
+  </si>
+  <si>
+    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von Glarner Kräuterkäse (Schabziger), FAM-Info. 432, 2002.</t>
+  </si>
+  <si>
+    <t>SwissMill, Produktinformationen Weizenmehl (Ruchmehl) Typ 1100, Zürich, Schweiz, 2008.</t>
+  </si>
+  <si>
+    <t>SwissMill, Produktinformationen Weizenmehl (Weissmehl) Typ 400, Zürich, Schweiz, 2008.</t>
+  </si>
+  <si>
+    <t>SwissMill, Produktinformationen Weizenmehl (Vollkornmehl) Typ 1700, Zürich, Schweiz, 2008.</t>
+  </si>
+  <si>
+    <t>Forschungsanstalt Agroscope Changins-Wädenswil ACW, Analysedaten Leadergemüse, Wädenswil, Schweiz, 2003.</t>
+  </si>
+  <si>
+    <t>Forschungsanstalt Agroscope Changins-Wädenswil ACW, Analysedaten Karotte, Wädenswil, Schweiz, 2004.</t>
+  </si>
+  <si>
+    <t>National Public Health Institute, Nutrition Unit. Fineli. Finnish food composition database. Release 11. Helsinki 2010. www.fineli.fi</t>
+  </si>
+  <si>
+    <t>Danish Food Composition Databank, version 7.0, 2008. www.foodcomp.dk</t>
+  </si>
+  <si>
+    <t>ISGEM, The Icelandic Food Composition Database, January 2011. www.matis.is/ISGEM/en/</t>
+  </si>
+  <si>
+    <t>Dutch Food Composition Database, NEVO online version 2010/2.0, RIVM, Bilthoven. www.rivm.nl/nevo_en/</t>
+  </si>
+  <si>
+    <t>Canadian Nutrient File, Version 2010. http://webprod.hc-sc.gc.ca/cnf-fce/index-eng.jsp</t>
+  </si>
+  <si>
+    <t>Souci Fachmann Kraut, Nährwertdatenbank, Garchung, Deutschland, January 2011. www.sfk-online.net/</t>
+  </si>
+  <si>
+    <t>U.S. Department of Agriculture, Agricultural Research Service. 2011. USDA National Nutrient Database for Standard Reference, Release 24. http://ndb.nal.usda.gov/</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2012</t>
+  </si>
+  <si>
+    <t>IG Dinkel, Laborbericht Urdinkelvollkornmehl, 2010</t>
+  </si>
+  <si>
+    <t>IG Dinkel, Laborbericht Urdinkelruchmehl, 2010</t>
+  </si>
+  <si>
+    <t>IG Dinkel, Laborbericht Urdinkelweissmehl, 2010</t>
+  </si>
+  <si>
+    <t>Saxholt, Christensen, Møller, Hartkopp, Hess Ygil, Hels: Danish Food Composition Databank, revision 7.1. Department of Nutrition, National Food Institute, Technical University of Denmark. 2009. www.foodcomp.dk/</t>
+  </si>
+  <si>
+    <t>Agence nationale de sécurité sanitaire de l'alimentation, de l'environment et du travail (anses), Table CIQUAL 2008 (www.afssa.fr/TableCIQUAL/)</t>
+  </si>
+  <si>
+    <t>Souci Fachmann Kraut, Die Zusammensetzung der Lebensmittel - Nährwert-Tabellen, 7. revidierte und ergänzte Auflage, Wissenschaftliche Verlagsgesellschaft mbH, 2008</t>
+  </si>
+  <si>
+    <t>Schmid et al. Die Zusammensetzung diverser Schweizer Rohpökelwaren. Fleischwirtschaft, 1: 84-88, 2011</t>
+  </si>
+  <si>
+    <t>Schmid et al. Die Zusammensetzung von Brühwürsten Schweizer Herkunft. Fleischwirtschaft, 10: 98-102, 2009</t>
+  </si>
+  <si>
+    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabelle Schweiz (Stand September 2011), www.mineralwasser.ch</t>
+  </si>
+  <si>
+    <t>Valser Mineralquellen, Mineralisierungstabellen der Valser Mineralquellen, Vals, Schweiz, 2011</t>
+  </si>
+  <si>
+    <t>Aproz Sources Minérales, Mineralisierung Mineralwasser, Aproz, Schweiz, 2012</t>
+  </si>
+  <si>
+    <t>Florin Switzerland, Produktinformation Schweizer HOLL-Rapsöl, 2012, www.florin-ag.ch</t>
+  </si>
+  <si>
+    <t>Sabo, Produktspezifikation Raffiniertes HO Sonnenblumenöl, 2012, www.sabo-oil.com</t>
+  </si>
+  <si>
+    <t>Pistor, Produktedeklarationsblatt HOLL Rapsöl, 2012, www.pistorone.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banca Dati di Composizione degli Alimenti per Studi epidemiologici in Italia BDA, 2008, www.ieo.it/bda2008/homepage.aspx </t>
+  </si>
+  <si>
+    <t>Schmid. Zusammensetzung von Fleischprodukten Schweizerischer Herkunft (Technisch-wissenschaftliche Informationen), ALP science Nr. 542, Agroscope Liebefeld-Posieux, 2012</t>
+  </si>
+  <si>
+    <t>The Norwegian Food Safety Authority, The Norwegian Directorate of Health and the University of Oslo. The Norwegian Food Composition Table 2012. www.matvaretabellen.no</t>
+  </si>
+  <si>
+    <t>Heineken Switzerland AG. Prüfberichte für Hubertus, Klosterbräu, Ittinger, Heineken Lager, Eichhof Lager und Calanda Lager. Chur, 2011</t>
+  </si>
+  <si>
+    <t>Heineken Switzerland AG. Alkohol- und Stammwürze-Gehalt von Heineken Lager, Calanda Lager, Eichhof Lager, Ittinger, Eichhof Klosterbräu und Eichhof Hubertus. Persönliche Kommunikation (Email vom 26.10.2011).</t>
+  </si>
+  <si>
+    <t>Pernod Ricard. Technical Product Specification (Malibu Coconut). Ontario, 2011</t>
+  </si>
+  <si>
+    <t>Pernod Ricard. Certificat produit  (Pastis de Marseille). Creteil Cedex, 2011</t>
+  </si>
+  <si>
+    <t>Pernod Ricard Italia. Certificate of analysis (Amaro Ramazzotti). Milano, 2011</t>
+  </si>
+  <si>
+    <t>Pernod Ricard. Certificat produit (Suze). Creteil Cedex, 2011</t>
+  </si>
+  <si>
+    <t>Sieber, R. Zusammensetzung von Milch und Milchprodukten Schweizerischer Herkunft (Technisch-wissenschaftliche Informationen). Agroscope Liebefeld-Posieux ALP. Bern, 2011. www.agroscope.admin.ch/data/publikationen/1314099178_as_538_web.pdf (2.8.2012)</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>Bundesamt für Gesundheit, Jod Monitoring, Bern, Schweiz, 2012</t>
+  </si>
+  <si>
+    <t>Bundesamt für Gesundheit, Jod Monitoring, Bern, Schweiz, 2011</t>
+  </si>
+  <si>
+    <t>Agence nationale de sécurité sanitaire de l'alimentation, de l'environment et du travail (anses), Table de composition nutritionnelle CIQUAL 2012 (www.afssa.fr/TableCIQUAL/)</t>
+  </si>
+  <si>
+    <t>Gerber, The role of meat in human nutrition for the supply with nutrients, particularly functional long-chain n-3 fatty acids, Dissertation (No. 17232), Eidgenössische Technische Hochschule, Zürich, 2007</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2014</t>
+  </si>
+  <si>
+    <t>Wauwiler Champignons AG, UFAG Prüfbericht Champignons geschnitten, Wauwil, Schweiz 2011</t>
+  </si>
+  <si>
+    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Speisesalz mit Iod und Fluor, Prattelen, Schweiz, 2014, www.salz.ch (16.1.2014)</t>
+  </si>
+  <si>
+    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Tafelsalz mit Iod, Prattelen, Schweiz, 2014, www.salz.ch (16.1.2014)</t>
+  </si>
+  <si>
+    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Speisesalz ohne Iod und Fluor, Prattelen, Schweiz, 2012, www.salz.ch (16.1.2014)</t>
+  </si>
+  <si>
+    <t>SwissMill, Spezifikation Halbweissmehl aus Weizen, Zürich, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>SwissMill, Spezifikation Ruchmehl aus Weizen, Zürich, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>SwissMill, Spezifikation Vollkornmehl aus Weizen, Zürich, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>SwissMill, Spezifikation Backmehl aus Weizen (Typ 550), Zürich, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>SwissMill, Spezifikation Weissmehl aus Weizen (Typ 400), Zürich, Schweiz, 2013</t>
+  </si>
+  <si>
+    <t>Thai Ministry of Public Health, Nutrition Division, Nutritive values of Thai foods, 2001</t>
+  </si>
+  <si>
+    <t>Presshefefabrik Stettfurt AG, UFAG Prüfbericht Backhefe Bio Knospe, Stettfurt, Schweiz, 2006</t>
+  </si>
+  <si>
+    <t>Food Composition Database of Sugiyama University, Standard Tables of Food Composition in Japan, 5th revised edition, 2000, http://database.food.sugiyama-u.ac.jp/index_asia.php</t>
+  </si>
+  <si>
+    <t>Morga AG, Produktinformation Agavensirup, Ebnat-Kappel, Schweiz, www.morga.ch (29.7.2014)</t>
+  </si>
+  <si>
+    <t>Eden Reform GmbH, Produktblatt Agavendicksaft, www.eden.de (29.7.2014)</t>
+  </si>
+  <si>
+    <t>Coop, Produktinformation zu Saitaku Wasabi Paste, www.coopathome (29.7.2014)</t>
+  </si>
+  <si>
+    <t>Blue Dragon UK, Blue Dragon Wasabi Paste, www.bluedragon.co.uk (29.7.2014)</t>
+  </si>
+  <si>
+    <t>Bundeslebensmittelschlüssel, BLS 3.02, Karlsruhe, Deutschland</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2015</t>
+  </si>
+  <si>
+    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Lebensmitteln für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2015</t>
+  </si>
+  <si>
+    <t>Bundesamt für Gesundheit, Selen Monitoring, Bern, Schweiz, 2010</t>
+  </si>
+  <si>
+    <t>U.S. Department of Agriculture, Agricultural Research Service. 2015. USDA National Nutrient Database for Standard Reference, Release 28. http://ndb.nal.usda.gov/</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2016</t>
+  </si>
+  <si>
+    <t>Sollberg H., Schaeren W., Collomb M., Badertscher R., Bütikofer U., Siber R., Beitrag zur Kenntnis der Zusammensetzung von Ziegenmilch schweizerischer Herkunft, ALP science Nr. 473, Agroscope Liebefeld-Posieux 2004</t>
+  </si>
+  <si>
+    <t>Maurer J., Schaeren W., Badertscher R., Bütikofer U., Collomb M., sieber R., Beitrag zur Kenntnis der Zusammensetzung von Schafmilch schweizerischer Herkunft, Mitt. Lebensm. Hyg. 97, Bern 2006</t>
+  </si>
+  <si>
+    <t>Souci Fachmann Kraut, Die Zusammensetzung der Lebensmittel - Nährwert-Tabellen, 8. revidierte und ergänzte Auflage, Wissenschaftliche Verlagsgesellschaft mbH, 2016</t>
+  </si>
+  <si>
+    <t>McCance and Widdowson's composition of foods integrated dataset, Public Health England, 2015</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Cerealien und Hülsenfrüchten für die Nährwertdatenbank (Analyseresultate), Épalinges , Schweiz, 2016</t>
+  </si>
+  <si>
+    <t>Table de composition nutritionnelle Ciqual (2016)</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2017</t>
+  </si>
+  <si>
+    <t>FAO. 2017. FAO/INFOODS Global Food Composition Database for Pulses Version 1.0 - uPulses1.0. Rome, FAO</t>
+  </si>
+  <si>
+    <t>U.S. Department of Agriculture, Agricultural Research Service, USDA National Nutrient Database for Standard Reference, Release 28 slightly revised May, 2016. http://ndb.nal.usda.gov/</t>
+  </si>
+  <si>
+    <t>Banca Dati di Composizione degli Alimenti per Studi epidemiologici in Italia BDA, 2015, http://www.bda-ieo.it/wordpress/</t>
+  </si>
+  <si>
+    <t>Frida Food Data (http://frida.fooddata.dk), version 2, 2016, National Food Institute, Technical University of Denmark</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Milch und Milchprodukte für die Nährwertdatenbank (Analyseresultate), Epalinges, Schweiz, 2017</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Käse für die Nährwertdatenbank (Analyseresultate), Epalinges, Schweiz, 2017</t>
+  </si>
+  <si>
+    <t>Anses - Table de composition nutritionnelle des aliments Ciqual 2017</t>
+  </si>
+  <si>
+    <t>Frida Food Data (http://frida.fooddata.dk), version 3, 2017, National Food Institute, Technical University of Denmark</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Fichier canadien sur les éléments nutritifs FCEN, 2015</t>
+  </si>
+  <si>
+    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Lebensmitteln für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Livsmedelsverket, Swedish National Food Agency food database, version 2017-12-15</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in oil and fat for swiss food composition database (analysis results), Epalinges, Switzerland, 2017</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in vegetables for swiss food composition database (analysis results), Epalinges, Switzerland, 2017-2018</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in potatoes for swiss food composition database (analysis results), Epalinges, Switzerland, 2017-2018</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in nuts for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
+  </si>
+  <si>
+    <t>Walther B, Wechsler D., Schlegel P., Haldimann M., Iodine in Swiss milk depending on production (conventional versus organic) and on processing (raw versus UHT) and the contribution of milk to the human iodine supply, Journal of Trace Elements in Medicine and Biology 46 (138-143), 2018</t>
+  </si>
+  <si>
+    <t>TürKomp, Turkish Food Composition Database, version 1.0. Food Institute, TÜBİTAK Marmara Research Center, Gebze / Kocaeli, 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geschätzter Wert / Valeur estimée / Valore stimato / Estimated value  </t>
+  </si>
+  <si>
+    <t>Berechneter Wert / valeur calculée / valore calcolato / calculated value</t>
+  </si>
+  <si>
+    <t>NEVO online version 2016/5.0, RIVM, Bilthoven. https://nevo-online.rivm.nl</t>
+  </si>
+  <si>
+    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabellen Schweiz (Stand January 2017) und Ausland (Stand Oktober 2017), www.mineralwasser.ch</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Datensammlung auf dem Schweizerlebensmittelmarkt, Bern, 2018</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in meat and eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Chicorée für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Apfel für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Rotkohl für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Rapsöl für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Karotten für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Vorzugsbutter für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2019</t>
+  </si>
+  <si>
+    <t>US Department of Agriculture (USDA), Agricultural Research Service, Nutrient Data Laboratory. USDA National Nutrient Database for Standard Reference, Legacy. Version Current: April 2018. Internet: http://www.ars.usda.gov/nutrientdata</t>
+  </si>
+  <si>
+    <t>Consorzio del Formaggio Parmigiano Reggiano, valori nutrizionali del Parmigiano Reggiano, website www.parmigianoreggiano.it, January 2019</t>
+  </si>
+  <si>
+    <t>Brunner K., Bestimmung von trockengehalt und Wassergehalt von Tofu-Produkten für Nährwertdatenbank (Analyseresultate), Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bern, Schweiz, 2019</t>
+  </si>
+  <si>
+    <t>Frida Food Data (http://frida.fooddata.dk), version 3a, 2018, National Food Institute, Technical University of Denmark</t>
+  </si>
+  <si>
+    <t>Public Health England, Nutrient analysis survey of fresh and processed fruit and vegetables with respect to fibre, analytical report, London 2017</t>
+  </si>
+  <si>
+    <t>Frida Food Data (http://frida.fooddata.dk), version 4, 2019, National Food Institute, Technical University of Denmark</t>
+  </si>
+  <si>
+    <t>McCance and Widdowson's composition of foods integrated dataset, Public Health England, 2019</t>
+  </si>
+  <si>
+    <t>Ministry of Education, Culture, Sports, Science and Technology (MEXT), Standard Tables of Food Composition in Japan, 7th revised edition, 2015</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
+  </si>
+  <si>
+    <t>Jakobsen J., Bysted A., Saxholt E., Wirenfeldt Nielsen C., Hess Ygil K. &amp; Trolle E., Næringsstofindhold i mel, gryn, kerner og frø, National Food Institute, Technical University of Denmark, 2019. www.food.dtu.dk</t>
+  </si>
+  <si>
+    <t>Kunchit Judprasong, Prapasri Puwastien, Nipa Rojroongwasinkul, Anadi Nitithamyong, Piyanut Sridonpai, Amnat Somjai. Institute of Nutrition, Mahidol University (2015). Thai Food Composition Database, Online version 2, September 2018, Thailand.  http://www.inmu.mahidol.ac.th/thaifcd</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Datensammlung auf dem Schweizerlebensmittelmarkt, Bern, 2019</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in Mustards for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
+  </si>
+  <si>
+    <t>FAO, Food and Agriculture Organization of the United Nations. West African Food Composition Table. Rome, 2012</t>
+  </si>
+  <si>
+    <t>National Institute for Health and Welfare, Public Health Promotion Unit. Fineli. Finnish food composition database. Release 20. Helsinki 2019. www.fineli.fi</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2020</t>
+  </si>
+  <si>
+    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen BLV, Trinkwasser Monitoring, Bern, Schweiz, 2020</t>
+  </si>
+  <si>
+    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Eiern für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2020</t>
+  </si>
+  <si>
+    <t>Infanger E, Haldimann M, Report on the composition of prevalent salt varieties, Federal Food Safety and Veterinary Office FSVO, Berne, Switzerland, 2016</t>
+  </si>
+  <si>
+    <t>Roe M., Pinchen H., Church S., Finglas P., Nutrient analysis of eggs, analytical report (revised version), Department of Health, 2013 https://www.gov.uk/government/publications/nutrient-analysis-of-eggs</t>
+  </si>
+  <si>
+    <t>Norwegian Food Composition Database 2019. Norwegian Food Safety Authority. www.matvaretabellen.no</t>
+  </si>
+  <si>
+    <t>Anses - Table de composition nutritionnelle des aliments Ciqual 2020</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in oil and fat, nuts and tofu for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2018-2021</t>
+  </si>
+  <si>
+    <t>Livsmedelsverket, The Swedish Food Agency food database, version 2020-01-16</t>
+  </si>
+  <si>
+    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabellen Schweiz und Ausland (Stand January 2020), www.mineralwasser.ch</t>
+  </si>
+  <si>
+    <t>T.Longvah, R. Ananthan, K. Bhaskarachary, K. Venkaiah, Indian Food Composition Tables, National institute of nutrition, India, 2017</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in vegetables for swiss food composition database (analysis results), Epalinges, Switzerland, 2018-2021</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2021</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in nuts and dried fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2020</t>
+  </si>
+  <si>
+    <t>Swiss Vitamin Institute, determination of vitamin in tofu and eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roe M., Pinchen H., Church S., Finglas P., Nutrient analysis of fruit and vegetables, analytical report, Department of Health, 2013 </t>
+  </si>
+  <si>
+    <t>NutriData food composition database, version 11.0. National Institute for Health Development 2021. tka.nutridata.ee</t>
+  </si>
+  <si>
+    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von Selen in Eiern für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2021</t>
+  </si>
+  <si>
+    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2022</t>
+  </si>
+  <si>
+    <t>Svarc O.L., Jensen M.B., Langwagen M., Poulsen A., Trolle E., Jakobsen J., 2022. Nutrient content in plant-based protein products intended for food composition databases. Journal of Food Composition and Analysis 106 (2022) 104332</t>
+  </si>
+  <si>
+    <t>Frida Food Data (http://frida.fooddata.dk), version 4.1, 2022, National Food Institute, Technical University of Denmark</t>
+  </si>
+  <si>
+    <t>Base de données suisse des valeurs nutritives – Aliments génériques V6.4 (13.06.2022)</t>
+  </si>
+  <si>
+    <t>Base de données suisse des valeurs nutritives – Produits de marque V6.4 (13.06.2022)</t>
+  </si>
+  <si>
+    <t>Base de données suisse des valeurs nutritives – Sources V6.4 (13.06.2022)</t>
+  </si>
+  <si>
+    <t>Rétinol (µg)</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lipides, totaux (g)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sel (NaCl) (g)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Eau minérale Volvic</t>
-  </si>
-  <si>
-    <t>Eau minérale Zurzacher</t>
-  </si>
-  <si>
-    <t>Eichhof Hubertus (bière spéciale brune, 6 vol%)</t>
-  </si>
-  <si>
-    <t>Energy drink, avec édulcorants (Moyenne de produits du commerce)</t>
-  </si>
-  <si>
-    <t>Ittinger (bière spéciale ambre, 5.6 vol%)</t>
-  </si>
-  <si>
-    <t>Malibu Coconut (21 vol%)</t>
-  </si>
-  <si>
-    <t>Pastis 51 de Marseille (45 vol%)</t>
-  </si>
-  <si>
-    <t>Sauce Worcester (Moyenne de produits du commerce)</t>
-  </si>
-  <si>
-    <t>Sucre vanillé (Moyenne de produits du commerce)</t>
-  </si>
-  <si>
-    <t>1662;1682</t>
-  </si>
-  <si>
-    <t>Suze (20 vol%)</t>
-  </si>
-  <si>
-    <t>Yogourt, à la grecque, avec crème, nature (Moyenne de produits du commerce)</t>
-  </si>
-  <si>
-    <t>Aargauer Zentralmolkerei AG, Suhr, Schweiz</t>
-  </si>
-  <si>
-    <t>Agroscope Liebefeld-Posieux, Liebefeld, Schweiz</t>
-  </si>
-  <si>
-    <t>Banca dati di composizione degli alimenti per studi epidemiologici in Italia</t>
-  </si>
-  <si>
-    <t>Bischofszell Nahrungsmittel AG, Bischofszell, Schweiz</t>
-  </si>
-  <si>
-    <t>Bundeslebensmittelschlüssel, BLS II.3.1, Karlsruhe, Deutschland</t>
-  </si>
-  <si>
-    <t>Bundeslebensmittelschlüssel, Karlsruhe, Deutschland</t>
-  </si>
-  <si>
-    <t>Canadian Nutrient File, version 2005. http://webprod.hc-sc.gc.ca/cnf-fce/start-debuter.do?lang=eng</t>
-  </si>
-  <si>
-    <t>Coop Schweiz, Zentrallabor, Pratteln, Schweiz</t>
-  </si>
-  <si>
-    <t>Danish food composition table</t>
-  </si>
-  <si>
-    <t>Emmi Schweiz AG, Emmen, Schweiz</t>
-  </si>
-  <si>
-    <t>Feldschlösschen Getränke AG, Rheinfelden, Schweiz</t>
-  </si>
-  <si>
-    <t>Haco AG, Gümlingen, Schweiz</t>
-  </si>
-  <si>
-    <t>Institut für Lebensmittel- und Ernährungswissenschaften, ETH Zürich, Schweiz 1</t>
-  </si>
-  <si>
-    <t>Institut für Lebensmittel- und Ernährungswissenschaften, ETH Zürich, Schweiz 2</t>
-  </si>
-  <si>
-    <t>Institut für Nutztierwissenschaften, ETH Zürich, Schweiz</t>
-  </si>
-  <si>
-    <t>Institute of Nutrition, Nakorn Pathom, Thailand</t>
-  </si>
-  <si>
-    <t>Kantonales Labor Zürich, Schweiz</t>
-  </si>
-  <si>
-    <t>Midor AG, Meilen, Schweiz</t>
-  </si>
-  <si>
-    <t>Mifa AG, Frenkendorf, Schweiz</t>
-  </si>
-  <si>
-    <t>Møller et al. Danish Food Composition Databank, revision 6.0. Food Informatics, Department of Nutrition, Danish Institute for Food and Veterinary Research. June 2005. www.foodcomp.dk/</t>
-  </si>
-  <si>
-    <t>Nährwerttabellen für Milch und Milchprodukte, Renner &amp; Renz-Schauen, Giessen, Deutschland</t>
-  </si>
-  <si>
-    <t>Nährwerttabellen, Souci Fachmann Kraut, Garching, Deutschland</t>
-  </si>
-  <si>
-    <t>Nestlé Suisse SA, Hirzel, Schweiz</t>
-  </si>
-  <si>
-    <t>Nestlé Suisse SA, Vevey, Schweiz</t>
-  </si>
-  <si>
-    <t>Nutrilait SA, Plan les Ouates, Schweiz</t>
-  </si>
-  <si>
-    <t>Répértoire général des aliments, Paris, Frankreich</t>
-  </si>
-  <si>
-    <t>Rivella AG, Rothrist, Schweiz</t>
-  </si>
-  <si>
-    <t>Schokoladefabriken Lindt &amp; Sprüngli AG, Produktinformationen Schokolade, Kilchberg, Schweiz, 2008.</t>
-  </si>
-  <si>
-    <t>Schweizerisches Vitamininstitut, Basel, Schweiz</t>
-  </si>
-  <si>
-    <t>Swiss Mill, Zürich, Schweiz</t>
-  </si>
-  <si>
-    <t>Swiss Quality Testing Services SQTS, Dietikon, Schweiz</t>
-  </si>
-  <si>
-    <t>SwissFIR, DAGRL, ETH Zürich, Schweiz</t>
-  </si>
-  <si>
-    <t>The composition of foods, McCance &amp; Widdowson</t>
-  </si>
-  <si>
-    <t>UFAG Laboratorien AG, Sursee, Schweiz</t>
-  </si>
-  <si>
-    <t>USDA National Nutrient Database for Standard Reference, Release 16, Beltsville, USA</t>
-  </si>
-  <si>
-    <t>USDA National Nutrient Database for Standard Reference, Release 19, Beltsville, USA. www.nal.usda.gov/fnic/foodcomp/search/</t>
-  </si>
-  <si>
-    <t>AFSSA/CIQUAL French food composition table version 2008. www.afssa.fr/TableCIQUAL/</t>
-  </si>
-  <si>
-    <t>Banca Dati di Composizione degli Alimenti INRAN, 2007. www.inran.it/646/tabelle_di_composizione_degli_alimenti.html</t>
-  </si>
-  <si>
-    <t>Barros et al. Chemical Composition and Biological Properties of Portuguese Wild Mushrooms: A Comprehensive Study. J. Agric. Food Chem. 56(10):3856-3862, 2008.</t>
-  </si>
-  <si>
-    <t>Borges et al. Nutritional quality of chestnut  (Castanea sativa Mill.) cultivars from Portugal. Food Chemistry 106:976-984, 2008.</t>
-  </si>
-  <si>
-    <t>Bureau et al. HPLC Determination of Carotenoids in Fruits and Vegetables in the United States. Journal of Food Science 51: 128-130, 1986.</t>
-  </si>
-  <si>
-    <t>Cabrera et al. Mineral content in legumes and nuts: contribution to the Spanish dietary intake. The science of the Total Enviroment 308:1-14, 2003.</t>
-  </si>
-  <si>
-    <t>Cardozo, Li. Total Dietary Fiber Content of Selected Nuts by Two Enzymatic-Gravimetric Methods. Journal of Food Composition and Analysis 7: 37-43, 1994.</t>
-  </si>
-  <si>
-    <t>De Oliveira, Rodriguez-Amaya. Processed and prepared corn products as sources of lutein and zeaxanthin: compositional variation in the food chain. J.Food Sci. 72(1):S79-S85, 2007.</t>
-  </si>
-  <si>
-    <t>Dias et al. Carotenoids in traditional Portuguese fruits and vegetables. Food Chemistry 113:808-815, 2009.</t>
-  </si>
-  <si>
-    <t>EL-Qudah. Identification and Quantification of Major Carotenoids in Some Vegetables. American Journal of Applied Sciences 6:492-497, 2009.</t>
-  </si>
-  <si>
-    <t>Food Composition Database for Epidemiological Studies in Italy by Gnagnarella P, Salvini S, Parpinel M. Version 1.2008, www.ieo.it/bda</t>
-  </si>
-  <si>
-    <t>Gambelli et al. Constituents of nutritional relevance in fermented milk products in Italy. Food Chemistry 66, 353-359, 1999.</t>
-  </si>
-  <si>
-    <t>Garcia-Linares et al. Microbiological and nutritional quality of sous vide or traditionally processed fish: Influence of fat content. J.Food Qual. 27(5):371-387, 2004.</t>
-  </si>
-  <si>
-    <t>Granado et al. Carotenoid composition in raw and cooked Spanish vegetables. Journal of Agriculture and Food Chemistry 40:2135-2140, 1992.</t>
-  </si>
-  <si>
-    <t>Haldimann et al. Iodine content of food groups. Journal of Food Composition and Analysis 18:461-471, 2005.</t>
-  </si>
-  <si>
-    <t>Hart et al. Development and evaluation of an HPLC method for the analysis of carotenoids in foods, measurement of carotenoid content of vegetables and fruits consumed in UK. Food Chemistry 54:101-111, 1995.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heinonen et al. Carotenoids in Finnish foods: vegetables, fruits, and berries. Journal of Food Composition and Analysis 37:655-659, 1989. </t>
-  </si>
-  <si>
-    <t>Heinonen et al. Carotenoids and retinoids in Finnish foods: cereal and bakery products. Cereal Chem. 66(4):270-273, 1989.</t>
-  </si>
-  <si>
-    <t>Heinonen et al. Carotenoids and retinoids in Finnish foods: dietary fats. J.Food Compos.Anal. 1(4):334-340, 1988.</t>
-  </si>
-  <si>
-    <t>Högberg et al. Muscle lipids, vitamins E and A, and lipid oxidation as affected by diet and RN genotype in female and castrated male Hampshire crossbreed pigs. Meat Science 60 (4):411-420, 2002.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holden et al. Carotenoid Content of U.S. Foods: An Update of the Database. Journal of Food Composition and Analysis 12:169-199, 1999. </t>
-  </si>
-  <si>
-    <t>Hoppner et al. Total Folate, Pantothenic Acid and Biotin Content of Yogurt Products, Can. Inst. Sci. Technol. J. , 23: 223-225, 1990</t>
-  </si>
-  <si>
-    <t>Hulshof et al. Variation in retinol and carotenoid content of milk and milk products in The Netherlands. Journal of Food Composition and Analysis 19:67-75, 2006.</t>
-  </si>
-  <si>
-    <t>Kandlakunta et al. Carotene content of some common (cereals, pulses, vegetables, spices and condiments) and unconventional sources of plant origin. Food Chem. 106(1):85-89, 2008.</t>
-  </si>
-  <si>
-    <t>Kessler, Morel. Vitamin A Konzentration in Kalbslebern: Eine Praxiserhebung. Agrarforschung 5 (5):225-227, 1998.</t>
-  </si>
-  <si>
-    <t>Köksal et al. Nutrient composition of hazelnut (Corylus avellana L.) varieties cultivated in Turkey. Food Chemistry 99:509-515, 2006.</t>
-  </si>
-  <si>
-    <t>Kornsteiner et al. Tocopherols and total phenolics in 10 different nut types. Food Chemistry 98:381-387, 2006.</t>
-  </si>
-  <si>
-    <t>Kumar, Aalbersberg. Nutrient retention in foods after earth-oven cooking compared to other forms of domestic cooking. 2. Vitamins. Journal of Food Composition and Analysis 19:311-320, 2006.</t>
-  </si>
-  <si>
-    <t>Kurz et al. HPLC-DAD-MS characterisation of carotenoids from apricots and pumpkins for the evaluation of fruit product authenticity. Food Chemistry 110:522-530, 2008.</t>
-  </si>
-  <si>
-    <t>Leonhardt et al. Vitamin E content of different animal products: Influence of animal nutrition. Zeitschrift für Ernährungswissenschaft 36:23-27, 1997.</t>
-  </si>
-  <si>
-    <t>Leonhardt, Wenk. Animal species and muscle related differences in thiamine and riboflavin contents of Swiss meat. Food Chemistry 59:449-452, 1997.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leth et al. The intake of carotenoids in Denmark. European Journal of Lipid Science Technology 128-132, 2000. </t>
-  </si>
-  <si>
-    <t>Livsmedelsdatabas - Swedish Food Composition Database, Schweden. Version: 07.10.2008</t>
-  </si>
-  <si>
-    <t>Lo Fiego et al. Effect of dietary supplementation of vitamins C and E in rabbits. Meat Science 67:319-327, 2004.</t>
-  </si>
-  <si>
-    <t>Lombardi-Boccia et al. Aspects of meat quality: trace elements and B vitamins in raw and cooked meats. Journal of Food Composition and Analysis 18:39-46, 2005.</t>
-  </si>
-  <si>
-    <t>Majchrzak et al. Vitamin A content (retinol and retinyl esters) in livers of different animals. Food Chem. 98(4):704-710, 2006.</t>
-  </si>
-  <si>
-    <t>Mangels et al. Carotenoid content of fruits and vegetables: An evaluation of analytic data. Journal American Dietetic Association 93:284-296, 1993.</t>
-  </si>
-  <si>
-    <t>Mattila et al. Contents of Cholecalciferol, Ergocalciferol, and Their 25-Hydroxylated Metabolites in Milk Products and Raw Meat and Liver As Determined by HPLC. Journal of Agriculture and Food Chemistry 43:2394-2399, 1995.</t>
-  </si>
-  <si>
-    <t>Moreiras et al. Tablas de composicion de alimentos, Piramide, 2005.</t>
-  </si>
-  <si>
-    <t>Müller et al. Determination of the carotenoid content in selected vegetabels and fruit by HPLC and photodiode array detection. Z. Lebensm. Unters. Forsch. A. 204:88-94, 1997.</t>
-  </si>
-  <si>
-    <t>Müller et al. Einfluss der Verarbeitung auf die Carotinoidgehalte von Gemüsesäften. Babynahrung und Tiefkühlprodukten, Deutsche Gesellschaft für Qualitätsforschung 155-160, 1997.</t>
-  </si>
-  <si>
-    <t>Müller. Die tägliche Aufnahme von Carotinoiden aus Gesamtnahrungsproben und die Carotinoidgehalte ausgewählter Gemüse-und Obstarten. Z. Ernährungswissenschaft 35:45-50, 1996.</t>
-  </si>
-  <si>
-    <t>Munzuroglu et al. The vitamin and selenium contents of apricot fruit of different verieties cultivated in different geographical regions. Food Chem. 83:205-212, 2003.</t>
-  </si>
-  <si>
-    <t>Murkovic et al. Development of an Austrian Carotenoid Database. Journal of Food Composition and Analysis 13:435-440, 2000.</t>
-  </si>
-  <si>
-    <t>Nährwerttabellen für Milch und Milchprodukte, Renner &amp; Renz-Schauen, Giessen, Deutschland, 1994</t>
-  </si>
-  <si>
-    <t>National Public Health Institute, Nutrition Unit. Fineli. Finnish food composition database. Release 9. Helsinki 2008. www.ktl.fi/fineli/</t>
-  </si>
-  <si>
-    <t>Niizu et al., New data on the carotenoid composition of raw salad vegetables. Journal of Food Composition and Analysis 18:739-749, 2005.</t>
-  </si>
-  <si>
-    <t>O'Neill et al. A European carotenoid database to assess carotenoid intakes and its use in five-country comparative study. British Journal of Nutrition 85:499-507, 2001.</t>
-  </si>
-  <si>
-    <t>Oliveira et al. Chemical composition, and antioxidant and antimicrobial activities of three hazelnut (Corylus avellana L.) cultivars. Food and Chemical Toxicology 46:1801-1807, 2008.</t>
-  </si>
-  <si>
-    <t>Olmedilla et al. Quantitation of provitamin-A and non-Provitamin-A carotenoids in the fruits most commonly consumed in Spain. Food and Cancer Prevention 141-145, 1993.</t>
-  </si>
-  <si>
-    <t>Orban et al. Nutritional quality and safety of whitefish (Coregonus lavaretus) from Italian lakes. J.Food Compos.Anal. 19(6-7):737-746, 2006.</t>
-  </si>
-  <si>
-    <t>Penã-Mendez et al. Characterization of various chestnut cultivars by means of chemometrics approach. Food Chemistry 107:537-544, 2008.</t>
-  </si>
-  <si>
-    <t>Plessi et al. Dietary Fiber and Some Elements in Nuts and Wheat Brans. Journal of Food Composition and Analysis 12:91-96, 1999.</t>
-  </si>
-  <si>
-    <t>Purchas et al. Concentrations of vitamin D3 and 25-hydroxyvitamin D3 in raw and cooked New Zealand beef and lamb. J.Food Compos.Anal. 20 (2):90-98, 2007.</t>
-  </si>
-  <si>
-    <t>Saxholt, Christensen, Møller, Hartkopp, Hess Ygil, Hels: Danish Food Composition Databank, revision 7. Department of Nutrition, National Food Institute, Technical University of Denmark. 2008. www.foodcomp.dk/</t>
-  </si>
-  <si>
-    <t>Schweizerische Nährwerttabelle für Fleisch und Fleischwaren. Wissenschaftliche Fassung.</t>
-  </si>
-  <si>
-    <t>Scott, Bishop. Nutrient Content of Milk and Milk Products: Vitamins of the B Complex and Vitamin C in Retail Creams, Ice Creams and Milk Shakes, J. Sci. Foood Agric., 1988</t>
-  </si>
-  <si>
-    <t>Setiawan et al. Carotenoid Content of Selected Indonesian Fruits. Journal of Food Composition and Analysis 14:169-176, 2001.</t>
-  </si>
-  <si>
-    <t>Singh et al. Antioxidant phytochemicals in cabbage (Brassica oleracea L. var. Capitata). Scientia Horticulturae 108:233-237, 2006.</t>
-  </si>
-  <si>
-    <t>Singh et al. Variability of carotenes, vitamin C, E and phenolics in Brassica vegetables. Journal of Food Composition and  Analysis 20:106-112, 2007.</t>
-  </si>
-  <si>
-    <t>Su et al. Identification and quantitation of major carotenoids in selected components of the Mediterranean diet: green leafy vegetables, figs and olive oil. European Journal of Clinical Nutrition 56:1149-1154, 2002.</t>
-  </si>
-  <si>
-    <t>SwissFIR, DAGRL, ETH Zürich, Inhaltsstoffe Wasser, berechnet aus Analysedaten der grössten Schweizer Wasserversorger, Schweiz, 2008.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Norwegian Food Safety Authority, The Norwegian Directorate of Health and the University of Oslo. The Norwegian Food Composition Table 2006. www.matportalen.no/matvaretabellen </t>
-  </si>
-  <si>
-    <t>U.S. Department of Agriculture, Agricultural Research Service. 2007. USDA National Nutrient Database for Standard Reference, Release 21. www.nal.usda.gov/fnic/foodcomp/search/</t>
-  </si>
-  <si>
-    <t>Van Heerden et al. Nutrient Content of South African Chickens. Journal of Food Composition and Analysis 15:47-64, 2002.</t>
-  </si>
-  <si>
-    <t>Van Heerden et al. The nutrient composition of South African lamb (A2 grade). Journal of Food Composition and Analysis 20:671-680, 2007.</t>
-  </si>
-  <si>
-    <t>Welna et al. Investigation of major and trace elements and their distributions between lipid and non-lipid fractions in Brazil nuts by inductively coupled plasma atomic optical spectrometry. Food Chemistry 111:1012-1015, 2008.</t>
-  </si>
-  <si>
-    <t>Williams et al. Composition of Australian red meat 2002. 3. Nutrient profile, Food Australia 59(7), 331-341, 2007.</t>
-  </si>
-  <si>
-    <t>Yano et al. Quantitation of Carotenoids in Raw and Processed Fruits in Japan. Food Sci. Technol. Res. 11:13-18, 2005.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Voll-, Halb- und Kaffeerahm, Mitt. Gebiete Lebensm. Hyg. 87:103-110, 1996.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer konsumreifer Emmentaler, Greyerzer, Sbrinz, Appenzeller und Tilsiter, Schweiz. Milchw. Forschung 17:109-118, 1988.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Joghurt, Mitt. Gebiete Lebensm. Hyg. 87:743-754, 1996.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer Milch, Mitt. Gebiete Lebensm. Hyg. 90:135-148, 1999.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischer Butter, Mitt. Gebiete Lebensm. Hyg. 89:84-96, 1998.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Quark und Hüttenkäse, Mitt. Gebiete Lebensm. Hyg. 90:662-669, 1999.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung schweizerischer konsumreifer Weich- und Halbhartkäse, Mitt. Gebierte Lebensm. Hyg. 85:366-381, 1994.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von schweizerischem Ziger, Mitt. Gebiete Lebensm. Hyg. 89:294-300, 1998.</t>
-  </si>
-  <si>
-    <t>Sieber et al. Beitrag zur Kenntnis der Zusammensetzung von Glarner Kräuterkäse (Schabziger), FAM-Info. 432, 2002.</t>
-  </si>
-  <si>
-    <t>SwissMill, Produktinformationen Weizenmehl (Ruchmehl) Typ 1100, Zürich, Schweiz, 2008.</t>
-  </si>
-  <si>
-    <t>SwissMill, Produktinformationen Weizenmehl (Weissmehl) Typ 400, Zürich, Schweiz, 2008.</t>
-  </si>
-  <si>
-    <t>SwissMill, Produktinformationen Weizenmehl (Vollkornmehl) Typ 1700, Zürich, Schweiz, 2008.</t>
-  </si>
-  <si>
-    <t>Forschungsanstalt Agroscope Changins-Wädenswil ACW, Analysedaten Leadergemüse, Wädenswil, Schweiz, 2003.</t>
-  </si>
-  <si>
-    <t>Forschungsanstalt Agroscope Changins-Wädenswil ACW, Analysedaten Karotte, Wädenswil, Schweiz, 2004.</t>
-  </si>
-  <si>
-    <t>National Public Health Institute, Nutrition Unit. Fineli. Finnish food composition database. Release 11. Helsinki 2010. www.fineli.fi</t>
-  </si>
-  <si>
-    <t>Danish Food Composition Databank, version 7.0, 2008. www.foodcomp.dk</t>
-  </si>
-  <si>
-    <t>ISGEM, The Icelandic Food Composition Database, January 2011. www.matis.is/ISGEM/en/</t>
-  </si>
-  <si>
-    <t>Dutch Food Composition Database, NEVO online version 2010/2.0, RIVM, Bilthoven. www.rivm.nl/nevo_en/</t>
-  </si>
-  <si>
-    <t>Canadian Nutrient File, Version 2010. http://webprod.hc-sc.gc.ca/cnf-fce/index-eng.jsp</t>
-  </si>
-  <si>
-    <t>Souci Fachmann Kraut, Nährwertdatenbank, Garchung, Deutschland, January 2011. www.sfk-online.net/</t>
-  </si>
-  <si>
-    <t>U.S. Department of Agriculture, Agricultural Research Service. 2011. USDA National Nutrient Database for Standard Reference, Release 24. http://ndb.nal.usda.gov/</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2012</t>
-  </si>
-  <si>
-    <t>IG Dinkel, Laborbericht Urdinkelvollkornmehl, 2010</t>
-  </si>
-  <si>
-    <t>IG Dinkel, Laborbericht Urdinkelruchmehl, 2010</t>
-  </si>
-  <si>
-    <t>IG Dinkel, Laborbericht Urdinkelweissmehl, 2010</t>
-  </si>
-  <si>
-    <t>Saxholt, Christensen, Møller, Hartkopp, Hess Ygil, Hels: Danish Food Composition Databank, revision 7.1. Department of Nutrition, National Food Institute, Technical University of Denmark. 2009. www.foodcomp.dk/</t>
-  </si>
-  <si>
-    <t>Agence nationale de sécurité sanitaire de l'alimentation, de l'environment et du travail (anses), Table CIQUAL 2008 (www.afssa.fr/TableCIQUAL/)</t>
-  </si>
-  <si>
-    <t>Souci Fachmann Kraut, Die Zusammensetzung der Lebensmittel - Nährwert-Tabellen, 7. revidierte und ergänzte Auflage, Wissenschaftliche Verlagsgesellschaft mbH, 2008</t>
-  </si>
-  <si>
-    <t>Schmid et al. Die Zusammensetzung diverser Schweizer Rohpökelwaren. Fleischwirtschaft, 1: 84-88, 2011</t>
-  </si>
-  <si>
-    <t>Schmid et al. Die Zusammensetzung von Brühwürsten Schweizer Herkunft. Fleischwirtschaft, 10: 98-102, 2009</t>
-  </si>
-  <si>
-    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabelle Schweiz (Stand September 2011), www.mineralwasser.ch</t>
-  </si>
-  <si>
-    <t>Valser Mineralquellen, Mineralisierungstabellen der Valser Mineralquellen, Vals, Schweiz, 2011</t>
-  </si>
-  <si>
-    <t>Aproz Sources Minérales, Mineralisierung Mineralwasser, Aproz, Schweiz, 2012</t>
-  </si>
-  <si>
-    <t>Florin Switzerland, Produktinformation Schweizer HOLL-Rapsöl, 2012, www.florin-ag.ch</t>
-  </si>
-  <si>
-    <t>Sabo, Produktspezifikation Raffiniertes HO Sonnenblumenöl, 2012, www.sabo-oil.com</t>
-  </si>
-  <si>
-    <t>Pistor, Produktedeklarationsblatt HOLL Rapsöl, 2012, www.pistorone.ch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banca Dati di Composizione degli Alimenti per Studi epidemiologici in Italia BDA, 2008, www.ieo.it/bda2008/homepage.aspx </t>
-  </si>
-  <si>
-    <t>Schmid. Zusammensetzung von Fleischprodukten Schweizerischer Herkunft (Technisch-wissenschaftliche Informationen), ALP science Nr. 542, Agroscope Liebefeld-Posieux, 2012</t>
-  </si>
-  <si>
-    <t>The Norwegian Food Safety Authority, The Norwegian Directorate of Health and the University of Oslo. The Norwegian Food Composition Table 2012. www.matvaretabellen.no</t>
-  </si>
-  <si>
-    <t>Heineken Switzerland AG. Prüfberichte für Hubertus, Klosterbräu, Ittinger, Heineken Lager, Eichhof Lager und Calanda Lager. Chur, 2011</t>
-  </si>
-  <si>
-    <t>Heineken Switzerland AG. Alkohol- und Stammwürze-Gehalt von Heineken Lager, Calanda Lager, Eichhof Lager, Ittinger, Eichhof Klosterbräu und Eichhof Hubertus. Persönliche Kommunikation (Email vom 26.10.2011).</t>
-  </si>
-  <si>
-    <t>Pernod Ricard. Technical Product Specification (Malibu Coconut). Ontario, 2011</t>
-  </si>
-  <si>
-    <t>Pernod Ricard. Certificat produit  (Pastis de Marseille). Creteil Cedex, 2011</t>
-  </si>
-  <si>
-    <t>Pernod Ricard Italia. Certificate of analysis (Amaro Ramazzotti). Milano, 2011</t>
-  </si>
-  <si>
-    <t>Pernod Ricard. Certificat produit (Suze). Creteil Cedex, 2011</t>
-  </si>
-  <si>
-    <t>Sieber, R. Zusammensetzung von Milch und Milchprodukten Schweizerischer Herkunft (Technisch-wissenschaftliche Informationen). Agroscope Liebefeld-Posieux ALP. Bern, 2011. www.agroscope.admin.ch/data/publikationen/1314099178_as_538_web.pdf (2.8.2012)</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>Bundesamt für Gesundheit, Jod Monitoring, Bern, Schweiz, 2012</t>
-  </si>
-  <si>
-    <t>Bundesamt für Gesundheit, Jod Monitoring, Bern, Schweiz, 2011</t>
-  </si>
-  <si>
-    <t>Agence nationale de sécurité sanitaire de l'alimentation, de l'environment et du travail (anses), Table de composition nutritionnelle CIQUAL 2012 (www.afssa.fr/TableCIQUAL/)</t>
-  </si>
-  <si>
-    <t>Gerber, The role of meat in human nutrition for the supply with nutrients, particularly functional long-chain n-3 fatty acids, Dissertation (No. 17232), Eidgenössische Technische Hochschule, Zürich, 2007</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2014</t>
-  </si>
-  <si>
-    <t>Wauwiler Champignons AG, UFAG Prüfbericht Champignons geschnitten, Wauwil, Schweiz 2011</t>
-  </si>
-  <si>
-    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Speisesalz mit Iod und Fluor, Prattelen, Schweiz, 2014, www.salz.ch (16.1.2014)</t>
-  </si>
-  <si>
-    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Tafelsalz mit Iod, Prattelen, Schweiz, 2014, www.salz.ch (16.1.2014)</t>
-  </si>
-  <si>
-    <t>Schweizer Rheinsalinen, Spezifikation für JuraSel Speisesalz ohne Iod und Fluor, Prattelen, Schweiz, 2012, www.salz.ch (16.1.2014)</t>
-  </si>
-  <si>
-    <t>SwissMill, Spezifikation Halbweissmehl aus Weizen, Zürich, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>SwissMill, Spezifikation Ruchmehl aus Weizen, Zürich, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>SwissMill, Spezifikation Vollkornmehl aus Weizen, Zürich, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>SwissMill, Spezifikation Backmehl aus Weizen (Typ 550), Zürich, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>SwissMill, Spezifikation Weissmehl aus Weizen (Typ 400), Zürich, Schweiz, 2013</t>
-  </si>
-  <si>
-    <t>Thai Ministry of Public Health, Nutrition Division, Nutritive values of Thai foods, 2001</t>
-  </si>
-  <si>
-    <t>Presshefefabrik Stettfurt AG, UFAG Prüfbericht Backhefe Bio Knospe, Stettfurt, Schweiz, 2006</t>
-  </si>
-  <si>
-    <t>Food Composition Database of Sugiyama University, Standard Tables of Food Composition in Japan, 5th revised edition, 2000, http://database.food.sugiyama-u.ac.jp/index_asia.php</t>
-  </si>
-  <si>
-    <t>Morga AG, Produktinformation Agavensirup, Ebnat-Kappel, Schweiz, www.morga.ch (29.7.2014)</t>
-  </si>
-  <si>
-    <t>Eden Reform GmbH, Produktblatt Agavendicksaft, www.eden.de (29.7.2014)</t>
-  </si>
-  <si>
-    <t>Coop, Produktinformation zu Saitaku Wasabi Paste, www.coopathome (29.7.2014)</t>
-  </si>
-  <si>
-    <t>Blue Dragon UK, Blue Dragon Wasabi Paste, www.bluedragon.co.uk (29.7.2014)</t>
-  </si>
-  <si>
-    <t>Bundeslebensmittelschlüssel, BLS 3.02, Karlsruhe, Deutschland</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2015</t>
-  </si>
-  <si>
-    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Lebensmitteln für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2015</t>
-  </si>
-  <si>
-    <t>Bundesamt für Gesundheit, Selen Monitoring, Bern, Schweiz, 2010</t>
-  </si>
-  <si>
-    <t>U.S. Department of Agriculture, Agricultural Research Service. 2015. USDA National Nutrient Database for Standard Reference, Release 28. http://ndb.nal.usda.gov/</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2016</t>
-  </si>
-  <si>
-    <t>Sollberg H., Schaeren W., Collomb M., Badertscher R., Bütikofer U., Siber R., Beitrag zur Kenntnis der Zusammensetzung von Ziegenmilch schweizerischer Herkunft, ALP science Nr. 473, Agroscope Liebefeld-Posieux 2004</t>
-  </si>
-  <si>
-    <t>Maurer J., Schaeren W., Badertscher R., Bütikofer U., Collomb M., sieber R., Beitrag zur Kenntnis der Zusammensetzung von Schafmilch schweizerischer Herkunft, Mitt. Lebensm. Hyg. 97, Bern 2006</t>
-  </si>
-  <si>
-    <t>Souci Fachmann Kraut, Die Zusammensetzung der Lebensmittel - Nährwert-Tabellen, 8. revidierte und ergänzte Auflage, Wissenschaftliche Verlagsgesellschaft mbH, 2016</t>
-  </si>
-  <si>
-    <t>McCance and Widdowson's composition of foods integrated dataset, Public Health England, 2015</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Cerealien und Hülsenfrüchten für die Nährwertdatenbank (Analyseresultate), Épalinges , Schweiz, 2016</t>
-  </si>
-  <si>
-    <t>Table de composition nutritionnelle Ciqual (2016)</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2017</t>
-  </si>
-  <si>
-    <t>FAO. 2017. FAO/INFOODS Global Food Composition Database for Pulses Version 1.0 - uPulses1.0. Rome, FAO</t>
-  </si>
-  <si>
-    <t>U.S. Department of Agriculture, Agricultural Research Service, USDA National Nutrient Database for Standard Reference, Release 28 slightly revised May, 2016. http://ndb.nal.usda.gov/</t>
-  </si>
-  <si>
-    <t>Banca Dati di Composizione degli Alimenti per Studi epidemiologici in Italia BDA, 2015, http://www.bda-ieo.it/wordpress/</t>
-  </si>
-  <si>
-    <t>Frida Food Data (http://frida.fooddata.dk), version 2, 2016, National Food Institute, Technical University of Denmark</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Milch und Milchprodukte für die Nährwertdatenbank (Analyseresultate), Epalinges, Schweiz, 2017</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, Bestimmung von Vitaminen in Käse für die Nährwertdatenbank (Analyseresultate), Epalinges, Schweiz, 2017</t>
-  </si>
-  <si>
-    <t>Anses - Table de composition nutritionnelle des aliments Ciqual 2017</t>
-  </si>
-  <si>
-    <t>Frida Food Data (http://frida.fooddata.dk), version 3, 2017, National Food Institute, Technical University of Denmark</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Fichier canadien sur les éléments nutritifs FCEN, 2015</t>
-  </si>
-  <si>
-    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Lebensmitteln für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Livsmedelsverket, Swedish National Food Agency food database, version 2017-12-15</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in oil and fat for swiss food composition database (analysis results), Epalinges, Switzerland, 2017</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in vegetables for swiss food composition database (analysis results), Epalinges, Switzerland, 2017-2018</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in potatoes for swiss food composition database (analysis results), Epalinges, Switzerland, 2017-2018</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in nuts for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
-  </si>
-  <si>
-    <t>Walther B, Wechsler D., Schlegel P., Haldimann M., Iodine in Swiss milk depending on production (conventional versus organic) and on processing (raw versus UHT) and the contribution of milk to the human iodine supply, Journal of Trace Elements in Medicine and Biology 46 (138-143), 2018</t>
-  </si>
-  <si>
-    <t>TürKomp, Turkish Food Composition Database, version 1.0. Food Institute, TÜBİTAK Marmara Research Center, Gebze / Kocaeli, 2014.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geschätzter Wert / Valeur estimée / Valore stimato / Estimated value  </t>
-  </si>
-  <si>
-    <t>Berechneter Wert / valeur calculée / valore calcolato / calculated value</t>
-  </si>
-  <si>
-    <t>NEVO online version 2016/5.0, RIVM, Bilthoven. https://nevo-online.rivm.nl</t>
-  </si>
-  <si>
-    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabellen Schweiz (Stand January 2017) und Ausland (Stand Oktober 2017), www.mineralwasser.ch</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Datensammlung auf dem Schweizerlebensmittelmarkt, Bern, 2018</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in meat and eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Chicorée für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Apfel für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Rotkohl für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Rapsöl für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Karotten für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Eurofins Scientific AG, Bestimmung von Vitaminen in Vorzugsbutter für die Nährwertdatenbank (Analyseresultate), Schönenwerd , Schweiz, 2018</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2019</t>
-  </si>
-  <si>
-    <t>US Department of Agriculture (USDA), Agricultural Research Service, Nutrient Data Laboratory. USDA National Nutrient Database for Standard Reference, Legacy. Version Current: April 2018. Internet: http://www.ars.usda.gov/nutrientdata</t>
-  </si>
-  <si>
-    <t>Consorzio del Formaggio Parmigiano Reggiano, valori nutrizionali del Parmigiano Reggiano, website www.parmigianoreggiano.it, January 2019</t>
-  </si>
-  <si>
-    <t>Brunner K., Bestimmung von trockengehalt und Wassergehalt von Tofu-Produkten für Nährwertdatenbank (Analyseresultate), Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bern, Schweiz, 2019</t>
-  </si>
-  <si>
-    <t>Frida Food Data (http://frida.fooddata.dk), version 3a, 2018, National Food Institute, Technical University of Denmark</t>
-  </si>
-  <si>
-    <t>Public Health England, Nutrient analysis survey of fresh and processed fruit and vegetables with respect to fibre, analytical report, London 2017</t>
-  </si>
-  <si>
-    <t>Frida Food Data (http://frida.fooddata.dk), version 4, 2019, National Food Institute, Technical University of Denmark</t>
-  </si>
-  <si>
-    <t>McCance and Widdowson's composition of foods integrated dataset, Public Health England, 2019</t>
-  </si>
-  <si>
-    <t>Ministry of Education, Culture, Sports, Science and Technology (MEXT), Standard Tables of Food Composition in Japan, 7th revised edition, 2015</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
-  </si>
-  <si>
-    <t>Jakobsen J., Bysted A., Saxholt E., Wirenfeldt Nielsen C., Hess Ygil K. &amp; Trolle E., Næringsstofindhold i mel, gryn, kerner og frø, National Food Institute, Technical University of Denmark, 2019. www.food.dtu.dk</t>
-  </si>
-  <si>
-    <t>Kunchit Judprasong, Prapasri Puwastien, Nipa Rojroongwasinkul, Anadi Nitithamyong, Piyanut Sridonpai, Amnat Somjai. Institute of Nutrition, Mahidol University (2015). Thai Food Composition Database, Online version 2, September 2018, Thailand.  http://www.inmu.mahidol.ac.th/thaifcd</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Datensammlung auf dem Schweizerlebensmittelmarkt, Bern, 2019</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in Mustards for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
-  </si>
-  <si>
-    <t>FAO, Food and Agriculture Organization of the United Nations. West African Food Composition Table. Rome, 2012</t>
-  </si>
-  <si>
-    <t>National Institute for Health and Welfare, Public Health Promotion Unit. Fineli. Finnish food composition database. Release 20. Helsinki 2019. www.fineli.fi</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2020</t>
-  </si>
-  <si>
-    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen BLV, Trinkwasser Monitoring, Bern, Schweiz, 2020</t>
-  </si>
-  <si>
-    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von mineralischen Elementen und Spurenelementen in Eiern für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2020</t>
-  </si>
-  <si>
-    <t>Infanger E, Haldimann M, Report on the composition of prevalent salt varieties, Federal Food Safety and Veterinary Office FSVO, Berne, Switzerland, 2016</t>
-  </si>
-  <si>
-    <t>Roe M., Pinchen H., Church S., Finglas P., Nutrient analysis of eggs, analytical report (revised version), Department of Health, 2013 https://www.gov.uk/government/publications/nutrient-analysis-of-eggs</t>
-  </si>
-  <si>
-    <t>Norwegian Food Composition Database 2019. Norwegian Food Safety Authority. www.matvaretabellen.no</t>
-  </si>
-  <si>
-    <t>Anses - Table de composition nutritionnelle des aliments Ciqual 2020</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in oil and fat, nuts and tofu for swiss food composition database (analysis results), Epalinges, Switzerland, 2019</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2018-2021</t>
-  </si>
-  <si>
-    <t>Livsmedelsverket, The Swedish Food Agency food database, version 2020-01-16</t>
-  </si>
-  <si>
-    <t>Verband Schweizerischer Mineralquellen und Soft-Drink-Produzenten SMS, Mineralisierungstabellen Schweiz und Ausland (Stand January 2020), www.mineralwasser.ch</t>
-  </si>
-  <si>
-    <t>T.Longvah, R. Ananthan, K. Bhaskarachary, K. Venkaiah, Indian Food Composition Tables, National institute of nutrition, India, 2017</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in vegetables for swiss food composition database (analysis results), Epalinges, Switzerland, 2018-2021</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2021</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in nuts and dried fruits for swiss food composition database (analysis results), Epalinges, Switzerland, 2020</t>
-  </si>
-  <si>
-    <t>Swiss Vitamin Institute, determination of vitamin in tofu and eggs for swiss food composition database (analysis results), Epalinges, Switzerland, 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roe M., Pinchen H., Church S., Finglas P., Nutrient analysis of fruit and vegetables, analytical report, Department of Health, 2013 </t>
-  </si>
-  <si>
-    <t>NutriData food composition database, version 11.0. National Institute for Health Development 2021. tka.nutridata.ee</t>
-  </si>
-  <si>
-    <t>Bundesamt für Lebensmittelsicherheit und Veterinärwesen, Bestimmung von Selen in Eiern für die Nährwertdatenbank (Analyseresultate), Bern, Schweiz, 2021</t>
-  </si>
-  <si>
-    <t>Schweizerische Gesellschaft für Ernährung SGE, Bern, Schweiz, 2022</t>
-  </si>
-  <si>
-    <t>Svarc O.L., Jensen M.B., Langwagen M., Poulsen A., Trolle E., Jakobsen J., 2022. Nutrient content in plant-based protein products intended for food composition databases. Journal of Food Composition and Analysis 106 (2022) 104332</t>
-  </si>
-  <si>
-    <t>Frida Food Data (http://frida.fooddata.dk), version 4.1, 2022, National Food Institute, Technical University of Denmark</t>
-  </si>
-  <si>
-    <t>Base de données suisse des valeurs nutritives – Aliments génériques V6.4 (13.06.2022)</t>
-  </si>
-  <si>
-    <t>Base de données suisse des valeurs nutritives – Produits de marque V6.4 (13.06.2022)</t>
-  </si>
-  <si>
-    <t>Base de données suisse des valeurs nutritives – Sources V6.4 (13.06.2022)</t>
-  </si>
-  <si>
-    <t>Rétinol (µg)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5458,8 +5471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB881A-4068-4DEA-B356-9AC1A56CFC86}">
   <dimension ref="A1:N1095"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5468,13 +5481,13 @@
     <col min="5" max="5" width="34.625" customWidth="1"/>
     <col min="6" max="6" width="35.625" customWidth="1"/>
     <col min="7" max="7" width="16.625" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="14" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" ht="177" x14ac:dyDescent="0.2">
@@ -5494,7 +5507,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>1674</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>45</v>
@@ -5509,10 +5522,10 @@
         <v>48</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>5</v>
+        <v>1675</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>15</v>
+        <v>1676</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>16</v>
@@ -45105,8 +45118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66102E2D-2934-4A87-8ECA-48276D87539B}">
   <dimension ref="A1:DY44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -45116,7 +45129,7 @@
   <sheetData>
     <row r="1" spans="1:129" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="3" spans="1:129" s="4" customFormat="1" ht="184.5" x14ac:dyDescent="0.2">
@@ -45298,7 +45311,7 @@
         <v>40</v>
       </c>
       <c r="BH3" s="3" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="BI3" s="3" t="s">
         <v>4</v>
@@ -54201,7 +54214,7 @@
         <v>1001070</v>
       </c>
       <c r="D34" t="s">
-        <v>1404</v>
+        <v>1677</v>
       </c>
       <c r="F34" t="s">
         <v>1381</v>
@@ -54548,7 +54561,7 @@
         <v>1001067</v>
       </c>
       <c r="D35" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="F35" t="s">
         <v>1381</v>
@@ -54886,7 +54899,7 @@
         <v>4088</v>
       </c>
       <c r="D36" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="F36" t="s">
         <v>165</v>
@@ -55092,7 +55105,7 @@
         <v>13436</v>
       </c>
       <c r="D37" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F37" t="s">
         <v>1210</v>
@@ -55307,7 +55320,7 @@
         <v>3563</v>
       </c>
       <c r="D38" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="F38" t="s">
         <v>165</v>
@@ -55513,7 +55526,7 @@
         <v>1262</v>
       </c>
       <c r="D39" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F39" t="s">
         <v>740</v>
@@ -55704,7 +55717,7 @@
         <v>1263</v>
       </c>
       <c r="D40" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="F40" t="s">
         <v>740</v>
@@ -55895,7 +55908,7 @@
         <v>13424</v>
       </c>
       <c r="D41" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="F41" t="s">
         <v>636</v>
@@ -56077,7 +56090,7 @@
         <v>13421</v>
       </c>
       <c r="D42" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="F42" t="s">
         <v>1205</v>
@@ -56113,7 +56126,7 @@
         <v>55</v>
       </c>
       <c r="T42" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="U42" t="s">
         <v>57</v>
@@ -56140,7 +56153,7 @@
         <v>55</v>
       </c>
       <c r="AI42" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="AJ42" t="s">
         <v>57</v>
@@ -56262,7 +56275,7 @@
         <v>1265</v>
       </c>
       <c r="D43" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="F43" t="s">
         <v>740</v>
@@ -56453,7 +56466,7 @@
         <v>13425</v>
       </c>
       <c r="D44" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F44" t="s">
         <v>1356</v>
@@ -56643,8 +56656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE56E702-7CFB-4BFB-BA7C-2624643189E0}">
   <dimension ref="A1:B258"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -56654,7 +56667,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -56670,7 +56683,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -56678,7 +56691,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -56686,7 +56699,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -56694,7 +56707,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -56702,7 +56715,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -56710,7 +56723,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -56718,7 +56731,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -56726,7 +56739,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -56734,7 +56747,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -56742,7 +56755,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -56750,7 +56763,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -56758,7 +56771,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -56766,7 +56779,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -56774,7 +56787,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -56782,7 +56795,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -56790,7 +56803,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -56798,7 +56811,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -56806,7 +56819,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -56814,7 +56827,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -56822,7 +56835,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -56830,7 +56843,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -56838,7 +56851,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -56846,7 +56859,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -56854,7 +56867,7 @@
         <v>38</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -56862,7 +56875,7 @@
         <v>41</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -56870,7 +56883,7 @@
         <v>43</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -56878,7 +56891,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -56886,7 +56899,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -56894,7 +56907,7 @@
         <v>47</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -56902,7 +56915,7 @@
         <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -56910,7 +56923,7 @@
         <v>50</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -56918,7 +56931,7 @@
         <v>51</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -56926,7 +56939,7 @@
         <v>53</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -56934,7 +56947,7 @@
         <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -56942,7 +56955,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -56950,7 +56963,7 @@
         <v>57</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -56958,7 +56971,7 @@
         <v>61</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -56966,7 +56979,7 @@
         <v>65</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -56974,7 +56987,7 @@
         <v>66</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -56982,7 +56995,7 @@
         <v>67</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -56990,7 +57003,7 @@
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -56998,7 +57011,7 @@
         <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -57006,7 +57019,7 @@
         <v>72</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -57014,7 +57027,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -57022,7 +57035,7 @@
         <v>75</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -57030,7 +57043,7 @@
         <v>78</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -57038,7 +57051,7 @@
         <v>81</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -57046,7 +57059,7 @@
         <v>83</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -57054,7 +57067,7 @@
         <v>84</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -57062,7 +57075,7 @@
         <v>87</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -57070,7 +57083,7 @@
         <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -57078,7 +57091,7 @@
         <v>89</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -57086,7 +57099,7 @@
         <v>90</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -57094,7 +57107,7 @@
         <v>91</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -57102,7 +57115,7 @@
         <v>92</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -57110,7 +57123,7 @@
         <v>94</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -57118,7 +57131,7 @@
         <v>95</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -57126,7 +57139,7 @@
         <v>97</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -57134,7 +57147,7 @@
         <v>98</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -57142,7 +57155,7 @@
         <v>99</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -57150,7 +57163,7 @@
         <v>100</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -57158,7 +57171,7 @@
         <v>102</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -57166,7 +57179,7 @@
         <v>103</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -57174,7 +57187,7 @@
         <v>104</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -57182,7 +57195,7 @@
         <v>105</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -57190,7 +57203,7 @@
         <v>107</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -57198,7 +57211,7 @@
         <v>108</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -57206,7 +57219,7 @@
         <v>109</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -57214,7 +57227,7 @@
         <v>110</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -57222,7 +57235,7 @@
         <v>111</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -57230,7 +57243,7 @@
         <v>112</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -57238,7 +57251,7 @@
         <v>115</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -57246,7 +57259,7 @@
         <v>116</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -57254,7 +57267,7 @@
         <v>117</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -57262,7 +57275,7 @@
         <v>120</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -57270,7 +57283,7 @@
         <v>121</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -57278,7 +57291,7 @@
         <v>122</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -57286,7 +57299,7 @@
         <v>123</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -57294,7 +57307,7 @@
         <v>124</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -57302,7 +57315,7 @@
         <v>125</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -57310,7 +57323,7 @@
         <v>127</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -57318,7 +57331,7 @@
         <v>128</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -57326,7 +57339,7 @@
         <v>130</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -57334,7 +57347,7 @@
         <v>131</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -57342,7 +57355,7 @@
         <v>132</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -57350,7 +57363,7 @@
         <v>134</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -57358,7 +57371,7 @@
         <v>136</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -57366,7 +57379,7 @@
         <v>137</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -57374,7 +57387,7 @@
         <v>141</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -57382,7 +57395,7 @@
         <v>143</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -57390,7 +57403,7 @@
         <v>145</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -57398,7 +57411,7 @@
         <v>146</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -57406,7 +57419,7 @@
         <v>147</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -57414,7 +57427,7 @@
         <v>149</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -57422,7 +57435,7 @@
         <v>150</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -57430,7 +57443,7 @@
         <v>151</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -57438,7 +57451,7 @@
         <v>152</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -57446,7 +57459,7 @@
         <v>153</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -57454,7 +57467,7 @@
         <v>155</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -57462,7 +57475,7 @@
         <v>156</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -57470,7 +57483,7 @@
         <v>159</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -57478,7 +57491,7 @@
         <v>160</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -57486,7 +57499,7 @@
         <v>162</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -57494,7 +57507,7 @@
         <v>163</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -57502,7 +57515,7 @@
         <v>164</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -57510,7 +57523,7 @@
         <v>176</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -57518,7 +57531,7 @@
         <v>177</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -57526,7 +57539,7 @@
         <v>178</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -57534,7 +57547,7 @@
         <v>181</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -57542,7 +57555,7 @@
         <v>182</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -57550,7 +57563,7 @@
         <v>183</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -57558,7 +57571,7 @@
         <v>184</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -57566,7 +57579,7 @@
         <v>185</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -57574,7 +57587,7 @@
         <v>186</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -57582,7 +57595,7 @@
         <v>311</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -57590,7 +57603,7 @@
         <v>312</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -57598,7 +57611,7 @@
         <v>315</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -57606,7 +57619,7 @@
         <v>318</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -57614,7 +57627,7 @@
         <v>319</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -57622,7 +57635,7 @@
         <v>993</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -57630,7 +57643,7 @@
         <v>994</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -57638,7 +57651,7 @@
         <v>996</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -57646,7 +57659,7 @@
         <v>998</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -57654,7 +57667,7 @@
         <v>999</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -57662,7 +57675,7 @@
         <v>1000</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -57670,7 +57683,7 @@
         <v>1002</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -57678,7 +57691,7 @@
         <v>1003</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -57686,7 +57699,7 @@
         <v>1004</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -57694,7 +57707,7 @@
         <v>1005</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -57702,7 +57715,7 @@
         <v>1006</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -57710,7 +57723,7 @@
         <v>1007</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -57718,7 +57731,7 @@
         <v>1008</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -57726,7 +57739,7 @@
         <v>1009</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -57734,7 +57747,7 @@
         <v>1010</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -57742,7 +57755,7 @@
         <v>1011</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -57750,7 +57763,7 @@
         <v>1013</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -57758,7 +57771,7 @@
         <v>1017</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
@@ -57766,7 +57779,7 @@
         <v>1025</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -57774,7 +57787,7 @@
         <v>1027</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -57782,7 +57795,7 @@
         <v>1028</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -57790,7 +57803,7 @@
         <v>1029</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -57798,7 +57811,7 @@
         <v>1030</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -57806,7 +57819,7 @@
         <v>1032</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -57814,7 +57827,7 @@
         <v>1033</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -57822,7 +57835,7 @@
         <v>1045</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -57830,7 +57843,7 @@
         <v>1047</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
@@ -57838,7 +57851,7 @@
         <v>1069</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
@@ -57846,7 +57859,7 @@
         <v>1070</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -57854,7 +57867,7 @@
         <v>1072</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -57862,7 +57875,7 @@
         <v>1073</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -57870,7 +57883,7 @@
         <v>1075</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -57878,7 +57891,7 @@
         <v>1129</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -57886,7 +57899,7 @@
         <v>1333</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -57894,7 +57907,7 @@
         <v>1399</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
@@ -57902,7 +57915,7 @@
         <v>1404</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
@@ -57910,7 +57923,7 @@
         <v>1406</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
@@ -57918,7 +57931,7 @@
         <v>1408</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
@@ -57926,7 +57939,7 @@
         <v>1410</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
@@ -57934,7 +57947,7 @@
         <v>1411</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
@@ -57942,7 +57955,7 @@
         <v>1412</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
@@ -57950,7 +57963,7 @@
         <v>1413</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
@@ -57958,7 +57971,7 @@
         <v>1438</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
@@ -57966,7 +57979,7 @@
         <v>1439</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
@@ -57974,7 +57987,7 @@
         <v>1440</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
@@ -57982,7 +57995,7 @@
         <v>1441</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -57990,7 +58003,7 @@
         <v>1442</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
@@ -57998,7 +58011,7 @@
         <v>1462</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
@@ -58006,7 +58019,7 @@
         <v>1463</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
@@ -58014,7 +58027,7 @@
         <v>1473</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
@@ -58022,7 +58035,7 @@
         <v>1476</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -58030,7 +58043,7 @@
         <v>1477</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
@@ -58038,7 +58051,7 @@
         <v>1480</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
@@ -58046,7 +58059,7 @@
         <v>1481</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
@@ -58054,7 +58067,7 @@
         <v>1528</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
@@ -58062,7 +58075,7 @@
         <v>1530</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -58070,7 +58083,7 @@
         <v>1542</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -58078,7 +58091,7 @@
         <v>1544</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -58086,7 +58099,7 @@
         <v>1631</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
@@ -58094,7 +58107,7 @@
         <v>1632</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
@@ -58102,7 +58115,7 @@
         <v>1637</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
@@ -58110,7 +58123,7 @@
         <v>1638</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
@@ -58118,7 +58131,7 @@
         <v>1640</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
@@ -58126,7 +58139,7 @@
         <v>1641</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
@@ -58134,7 +58147,7 @@
         <v>1642</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
@@ -58142,7 +58155,7 @@
         <v>1643</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
@@ -58150,7 +58163,7 @@
         <v>1648</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
@@ -58158,7 +58171,7 @@
         <v>1649</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -58166,7 +58179,7 @@
         <v>1650</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
@@ -58174,7 +58187,7 @@
         <v>1651</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
@@ -58182,7 +58195,7 @@
         <v>1652</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
@@ -58190,7 +58203,7 @@
         <v>1653</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
@@ -58198,7 +58211,7 @@
         <v>1659</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
@@ -58206,7 +58219,7 @@
         <v>1660</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
@@ -58214,7 +58227,7 @@
         <v>1661</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
@@ -58222,7 +58235,7 @@
         <v>1662</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
@@ -58230,7 +58243,7 @@
         <v>1663</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
@@ -58238,7 +58251,7 @@
         <v>1665</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
@@ -58246,7 +58259,7 @@
         <v>1666</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
@@ -58254,7 +58267,7 @@
         <v>1667</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
@@ -58262,7 +58275,7 @@
         <v>1669</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
@@ -58270,7 +58283,7 @@
         <v>1670</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
@@ -58278,7 +58291,7 @@
         <v>1671</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
@@ -58286,7 +58299,7 @@
         <v>1672</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
@@ -58294,7 +58307,7 @@
         <v>1675</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
@@ -58302,7 +58315,7 @@
         <v>1676</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
@@ -58310,7 +58323,7 @@
         <v>1677</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
@@ -58318,7 +58331,7 @@
         <v>1678</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
@@ -58326,7 +58339,7 @@
         <v>1679</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
@@ -58334,7 +58347,7 @@
         <v>1680</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
@@ -58342,7 +58355,7 @@
         <v>1682</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
@@ -58350,7 +58363,7 @@
         <v>1690</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
@@ -58358,7 +58371,7 @@
         <v>1691</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
@@ -58366,7 +58379,7 @@
         <v>1692</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
@@ -58374,7 +58387,7 @@
         <v>1693</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
@@ -58382,7 +58395,7 @@
         <v>1694</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
@@ -58390,7 +58403,7 @@
         <v>1696</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
@@ -58398,7 +58411,7 @@
         <v>1697</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
@@ -58406,7 +58419,7 @@
         <v>1698</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
@@ -58414,7 +58427,7 @@
         <v>1699</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
@@ -58422,7 +58435,7 @@
         <v>1700</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
@@ -58430,7 +58443,7 @@
         <v>1703</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
@@ -58438,7 +58451,7 @@
         <v>1704</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
@@ -58446,7 +58459,7 @@
         <v>1705</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
@@ -58454,7 +58467,7 @@
         <v>2238</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
@@ -58462,7 +58475,7 @@
         <v>2239</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
@@ -58470,7 +58483,7 @@
         <v>2240</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
@@ -58478,7 +58491,7 @@
         <v>2241</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
@@ -58486,7 +58499,7 @@
         <v>2242</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
@@ -58494,7 +58507,7 @@
         <v>2243</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
@@ -58502,7 +58515,7 @@
         <v>2245</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
@@ -58510,7 +58523,7 @@
         <v>2247</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
@@ -58518,7 +58531,7 @@
         <v>2252</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
@@ -58526,7 +58539,7 @@
         <v>2256</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
@@ -58534,7 +58547,7 @@
         <v>2265</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
@@ -58542,7 +58555,7 @@
         <v>2268</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
@@ -58550,7 +58563,7 @@
         <v>2269</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
@@ -58558,7 +58571,7 @@
         <v>2272</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
@@ -58566,7 +58579,7 @@
         <v>2275</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
@@ -58574,7 +58587,7 @@
         <v>2276</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
@@ -58582,7 +58595,7 @@
         <v>2277</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
@@ -58590,7 +58603,7 @@
         <v>2278</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
@@ -58598,7 +58611,7 @@
         <v>2279</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
@@ -58606,7 +58619,7 @@
         <v>2283</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
@@ -58614,7 +58627,7 @@
         <v>2289</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
@@ -58622,7 +58635,7 @@
         <v>2290</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
@@ -58630,7 +58643,7 @@
         <v>2579</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
@@ -58638,7 +58651,7 @@
         <v>2580</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
@@ -58646,7 +58659,7 @@
         <v>2581</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
@@ -58654,7 +58667,7 @@
         <v>2597</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
@@ -58662,7 +58675,7 @@
         <v>2598</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
@@ -58670,7 +58683,7 @@
         <v>2600</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
@@ -58678,7 +58691,7 @@
         <v>2602</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
@@ -58686,7 +58699,7 @@
         <v>2603</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
@@ -58694,7 +58707,7 @@
         <v>2606</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
@@ -58702,7 +58715,7 @@
         <v>2608</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>